<commit_message>
Updated BOM of the front panel.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/stepper driver front panel/stepperdriver front panel BOM.xlsx
+++ b/Hardware/PCB/stepper driver front panel/stepperdriver front panel BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\harp-tech\device.stepperdriver\Hardware\PCB\stepper driver front panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{68BC23AC-90A6-4742-B5C4-49654BEBDF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953B4682-463F-464D-B693-8BE8F81CB1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stepperdriver front panel" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Reference(s)</t>
   </si>
@@ -64,21 +64,12 @@
     <t>R1</t>
   </si>
   <si>
-    <t>RESISTOR: SMD 0603 0? 1A [RC0603FR-070RL] [SMD]</t>
-  </si>
-  <si>
     <t>RC0603FR-070RL</t>
   </si>
   <si>
     <t>OEPS020079</t>
   </si>
   <si>
-    <t>R2, R5, R6, R7, R8, R9, R10, R11</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -107,12 +98,42 @@
   </si>
   <si>
     <t>OEPS070054</t>
+  </si>
+  <si>
+    <t>R2, R5, R6, R7</t>
+  </si>
+  <si>
+    <t>R8, R9, R10, R11</t>
+  </si>
+  <si>
+    <t>OEPS020013</t>
+  </si>
+  <si>
+    <t>RESISTOR: SMD 0603 0Ω 1A [RC0603FR-070RL] [SMD]</t>
+  </si>
+  <si>
+    <t>RESISTOR: SMD 0402 10kΩ ±1% 0.100W [ERJ-2RKF1002X] [SMD]</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1002X</t>
+  </si>
+  <si>
+    <t>OEPS090005</t>
+  </si>
+  <si>
+    <t>CABLE: FFC / FPC 26WAY 0.5MM 152MM [MP-FFCA05261522A]</t>
+  </si>
+  <si>
+    <t>MP-FFCA05261522A</t>
+  </si>
+  <si>
+    <t>POST-PRODUCTION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -957,17 +978,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1017,78 +1041,112 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>